<commit_message>
Embedded matplotlib plots into the tkinter window
</commit_message>
<xml_diff>
--- a/outputs/first_order_ode.xlsx
+++ b/outputs/first_order_ode.xlsx
@@ -375,154 +375,154 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.2105263157894737</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="B3">
-        <v>1.210526315789474</v>
+        <v>1.105263157894737</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.4210526315789473</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="B4">
-        <v>1.465373961218837</v>
+        <v>1.221606648199446</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.631578947368421</v>
+        <v>0.3157894736842105</v>
       </c>
       <c r="B5">
-        <v>1.773873742528065</v>
+        <v>1.350196821694124</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.8421052631578947</v>
+        <v>0.4210526315789473</v>
       </c>
       <c r="B6">
-        <v>2.147320846218184</v>
+        <v>1.492322802925085</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>1.052631578947368</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="B7">
-        <v>2.599388392790433</v>
+        <v>1.649409413759304</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>1.263157894736842</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="B8">
-        <v>3.146628054430525</v>
+        <v>1.823031457312915</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>1.473684210526316</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="B9">
-        <v>3.809076065889583</v>
+        <v>2.014929505451117</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>1.684210526315789</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="B10">
-        <v>4.610986816603179</v>
+        <v>2.227027348130182</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>1.894736842105263</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="B11">
-        <v>5.58172088325648</v>
+        <v>2.461451279512306</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>2.105263157894737</v>
+        <v>1.052631578947368</v>
       </c>
       <c r="B12">
-        <v>6.756820016573634</v>
+        <v>2.720551414197812</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>2.315789473684211</v>
+        <v>1.157894736842105</v>
       </c>
       <c r="B13">
-        <v>8.179308441115452</v>
+        <v>3.006925247271266</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>2.526315789473684</v>
+        <v>1.263157894736842</v>
       </c>
       <c r="B14">
-        <v>9.901268112929232</v>
+        <v>3.323443694352452</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>2.736842105263158</v>
+        <v>1.368421052631579</v>
       </c>
       <c r="B15">
-        <v>11.98574561038802</v>
+        <v>3.673279872705341</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>2.947368421052631</v>
+        <v>1.473684210526316</v>
       </c>
       <c r="B16">
-        <v>14.50906047573286</v>
+        <v>4.059940911937482</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>3.157894736842105</v>
+        <v>1.578947368421053</v>
       </c>
       <c r="B17">
-        <v>17.56359952325557</v>
+        <v>4.487303113194059</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>3.368421052631579</v>
+        <v>1.684210526315789</v>
       </c>
       <c r="B18">
-        <v>21.26119942288832</v>
+        <v>4.95965080931975</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>3.578947368421052</v>
+        <v>1.789473684210526</v>
       </c>
       <c r="B19">
-        <v>25.73724140665428</v>
+        <v>5.481719315563934</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>3.789473684210526</v>
+        <v>1.894736842105263</v>
       </c>
       <c r="B20">
-        <v>31.1556080185815</v>
+        <v>6.058742401412769</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B21">
-        <v>37.71468339091445</v>
+        <v>6.696504759456219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>